<commit_message>
code changes in Excel Manager
</commit_message>
<xml_diff>
--- a/PageObjectModel/src/test/resources/TestData/CalculaterTestData.xlsx
+++ b/PageObjectModel/src/test/resources/TestData/CalculaterTestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43C8B44-0F6F-41B1-ACFC-918048EC9971}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Mortgage Amount</t>
   </si>
@@ -61,17 +62,20 @@
   </si>
   <si>
     <t>Variable</t>
+  </si>
+  <si>
+    <t>Test Result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,8 +90,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,6 +118,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -110,17 +133,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -212,6 +238,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -247,6 +290,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -422,28 +482,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,8 +538,11 @@
       <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="L1" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>500000</v>
       </c>
@@ -513,7 +577,7 @@
         <v>2608.2399999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1000000</v>
       </c>
@@ -548,7 +612,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2000000</v>
       </c>
@@ -583,7 +647,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10000000</v>
       </c>
@@ -625,24 +689,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>